<commit_message>
Deskripsi perubahan yang jelas
</commit_message>
<xml_diff>
--- a/data/Data_Pendaftaran.xlsx
+++ b/data/Data_Pendaftaran.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="32">
   <si>
     <t>No</t>
   </si>
@@ -74,16 +74,40 @@
     <t/>
   </si>
   <si>
-    <t>Kumite</t>
+    <t>Kata</t>
   </si>
   <si>
     <t>Festival</t>
   </si>
   <si>
-    <t>Festival Kumite Under-21 -55kg Putra</t>
-  </si>
-  <si>
-    <t>20/6/2025, 14.59.52</t>
+    <t>FESTIVAL KATA PERORANGAN UNDER-21 SABUK HITAM PUTRA</t>
+  </si>
+  <si>
+    <t>25/6/2025, 00.35.43</t>
+  </si>
+  <si>
+    <t>Fikrul cs</t>
+  </si>
+  <si>
+    <t>Kata Beregu</t>
+  </si>
+  <si>
+    <t>Prestasi</t>
+  </si>
+  <si>
+    <t>KATA BEREGU UNDER-21 PUTRA</t>
+  </si>
+  <si>
+    <t>25/6/2025, 00.36.09</t>
+  </si>
+  <si>
+    <t>KATA PERORANGAN UNDER-21 PUTRA</t>
+  </si>
+  <si>
+    <t>25/6/2025, 00.36.22</t>
+  </si>
+  <si>
+    <t>25/6/2025, 00.42.45</t>
   </si>
 </sst>
 </file>
@@ -111,7 +135,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor rgb="FFFF99"/>
       </patternFill>
     </fill>
   </fills>
@@ -127,13 +151,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -477,17 +504,15 @@
   <dimension ref="A1:M2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="1" width="5" customWidth="1"/>
-    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="1" max="1" width="3.5" customWidth="1"/>
+    <col min="2" max="2" width="35" customWidth="1"/>
     <col min="3" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="6" width="25" customWidth="1"/>
-    <col min="7" max="7" width="12" customWidth="1"/>
-    <col min="8" max="8" width="10" customWidth="1"/>
-    <col min="9" max="9" width="20" customWidth="1"/>
-    <col min="10" max="10" width="18" customWidth="1"/>
-    <col min="11" max="11" width="20" customWidth="1"/>
-    <col min="12" max="12" width="30" customWidth="1"/>
+    <col min="5" max="5" width="13" customWidth="1"/>
+    <col min="6" max="6" width="20" customWidth="1"/>
+    <col min="7" max="7" width="10" customWidth="1"/>
+    <col min="8" max="8" width="8" customWidth="1"/>
+    <col min="9" max="11" width="20" customWidth="1"/>
+    <col min="12" max="12" width="60" customWidth="1"/>
     <col min="13" max="13" width="25" customWidth="1"/>
   </cols>
   <sheetData>
@@ -555,7 +580,7 @@
         <v>18</v>
       </c>
       <c r="H2" s="2">
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>19</v>
@@ -566,7 +591,7 @@
       <c r="K2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="3" t="s">
         <v>22</v>
       </c>
       <c r="M2" s="2" t="s">
@@ -581,20 +606,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:M4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="1" width="5" customWidth="1"/>
-    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="1" max="1" width="3.5" customWidth="1"/>
+    <col min="2" max="2" width="35" customWidth="1"/>
     <col min="3" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="6" width="25" customWidth="1"/>
-    <col min="7" max="7" width="12" customWidth="1"/>
-    <col min="8" max="8" width="10" customWidth="1"/>
-    <col min="9" max="9" width="20" customWidth="1"/>
-    <col min="10" max="10" width="18" customWidth="1"/>
-    <col min="11" max="11" width="20" customWidth="1"/>
-    <col min="12" max="12" width="30" customWidth="1"/>
+    <col min="5" max="5" width="13" customWidth="1"/>
+    <col min="6" max="6" width="20" customWidth="1"/>
+    <col min="7" max="7" width="10" customWidth="1"/>
+    <col min="8" max="8" width="8" customWidth="1"/>
+    <col min="9" max="11" width="20" customWidth="1"/>
+    <col min="12" max="12" width="60" customWidth="1"/>
     <col min="13" max="13" width="25" customWidth="1"/>
   </cols>
   <sheetData>
@@ -639,6 +662,129 @@
         <v>12</v>
       </c>
     </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>